<commit_message>
Rewritting all the ASHRAE CE100-200
</commit_message>
<xml_diff>
--- a/ASHRAE_140/COOLING_TEST/HVAC_equipments/HVAC_DX_equipment_CE100.xlsx
+++ b/ASHRAE_140/COOLING_TEST/HVAC_equipments/HVAC_DX_equipment_CE100.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jfc/Disco Google/INVESTIGA/OPENSIMULA/HVAC_Equipments/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jfc/Documents/OpenSimula/ASHRAE_140/COOLING_TEST/HVAC_equipments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE318F1-90CC-B648-BEBB-A94A67BC39DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07BE29C2-2243-CA4D-B01A-27F629923220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2500" yWindow="2760" windowWidth="38080" windowHeight="20780" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44400" yWindow="2380" windowWidth="38080" windowHeight="20780" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ASHRAE-140 Case CE100" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="36">
   <si>
     <t>HVAC_DX_equipment</t>
   </si>
@@ -127,6 +127,24 @@
     <t>c_9</t>
   </si>
   <si>
+    <t>indoor_fan</t>
+  </si>
+  <si>
+    <t>Q_tot_net</t>
+  </si>
+  <si>
+    <t>P_comp</t>
+  </si>
+  <si>
+    <t>P_tot</t>
+  </si>
+  <si>
+    <t>Compressor + outdoor fan</t>
+  </si>
+  <si>
+    <t>Q_sen_net</t>
+  </si>
+  <si>
     <t>P</t>
   </si>
 </sst>
@@ -138,7 +156,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -148,7 +166,7 @@
     <font>
       <sz val="12"/>
       <name val="Helvetica Neue"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -156,8 +174,19 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF3B3B3B"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -168,6 +197,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -183,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -194,6 +229,11 @@
     <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -321,10 +361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:O24"/>
+  <dimension ref="B2:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C30" sqref="C29:O30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -409,7 +449,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="2">
-        <v>7951.3293290360398</v>
+        <v>8181</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>10</v>
@@ -420,7 +460,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="2">
-        <v>6134.7456782889003</v>
+        <v>6365</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>10</v>
@@ -431,191 +471,207 @@
         <v>12</v>
       </c>
       <c r="C14" s="1">
-        <f>1858+230+108</f>
-        <v>2196</v>
+        <v>1966</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B16" s="1" t="s">
+      <c r="E14" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B15" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="1">
+        <v>230</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="C18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="1" t="s">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="I19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B19" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="1">
-        <v>9.0990418100000004E-4</v>
-      </c>
-      <c r="D19" s="1">
-        <v>4.3508074299999998E-2</v>
-      </c>
-      <c r="E19" s="1">
-        <v>-3.4751605899999999E-5</v>
-      </c>
-      <c r="F19" s="1">
-        <v>1.5124703800000001E-4</v>
-      </c>
-      <c r="G19" s="1">
-        <v>-4.7034572900000001E-4</v>
-      </c>
-      <c r="H19" s="1">
-        <v>0.42808307899999998</v>
-      </c>
-      <c r="I19" s="1">
-        <v>0.99983654300000002</v>
-      </c>
-      <c r="K19" s="1">
-        <f>C19*C8+D19*C7+E19*C8^2+F19*C7^2+G19*C8*C7+H19</f>
-        <v>0.99897423475817992</v>
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" s="1">
-        <v>1.19823328E-2</v>
-      </c>
-      <c r="D20" s="1">
-        <v>1.43238759E-2</v>
+        <v>23</v>
+      </c>
+      <c r="C20" s="14">
+        <v>8.8432320599999995E-4</v>
+      </c>
+      <c r="D20" s="14">
+        <v>4.22848917E-2</v>
       </c>
       <c r="E20" s="1">
-        <v>5.6562546200000002E-5</v>
-      </c>
-      <c r="F20" s="1">
-        <v>3.7245239300000002E-5</v>
-      </c>
-      <c r="G20" s="1">
-        <v>-1.84024752E-4</v>
-      </c>
-      <c r="H20" s="1">
-        <v>0.34541167</v>
-      </c>
-      <c r="I20" s="1">
-        <v>0.99954382100000005</v>
+        <v>-3.4751605899999999E-5</v>
+      </c>
+      <c r="F20" s="14">
+        <v>1.4699489E-4</v>
+      </c>
+      <c r="G20" s="14">
+        <v>-4.57122466E-4</v>
+      </c>
+      <c r="H20" s="14">
+        <v>0.44416190700000002</v>
+      </c>
+      <c r="I20" s="14">
+        <v>0.99983654300000002</v>
       </c>
       <c r="K20" s="1">
         <f>C20*C8+D20*C7+E20*C8^2+F20*C7^2+G20*C8*C7+H20</f>
-        <v>1.001030441209948</v>
-      </c>
-    </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="C22" s="1" t="s">
-        <v>24</v>
+        <v>0.99780624334890011</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="14">
+        <v>1.3384131699999999E-2</v>
+      </c>
+      <c r="D21" s="14">
+        <v>1.5999609099999999E-2</v>
+      </c>
+      <c r="E21" s="14">
+        <v>6.3179731200000002E-5</v>
+      </c>
+      <c r="F21" s="14">
+        <v>4.1602515499999999E-5</v>
+      </c>
+      <c r="G21" s="14">
+        <v>-2.0555358900000001E-4</v>
+      </c>
+      <c r="H21" s="14">
+        <v>0.26883215999999999</v>
+      </c>
+      <c r="I21" s="14">
+        <v>0.99954382100000005</v>
+      </c>
+      <c r="K21" s="1">
+        <f>C21*C8+D21*C7+E21*C8^2+F21*C7^2+G21*C8*C7+H21</f>
+        <v>1.0011509925625801</v>
       </c>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C23" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D23" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="H24" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="I24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J23" s="1" t="s">
+      <c r="J24" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="K23" s="1" t="s">
+      <c r="K24" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L23" s="1" t="s">
+      <c r="L24" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="M23" s="1" t="s">
+      <c r="M24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="O23" s="1" t="s">
+      <c r="O24" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B24" s="1" t="s">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="1">
-        <v>1.1479779699999999E-3</v>
-      </c>
-      <c r="D24" s="1">
-        <v>-7.8858117800000002E-2</v>
-      </c>
-      <c r="E24" s="1">
-        <v>0.10443063900000001</v>
-      </c>
-      <c r="F24" s="1">
-        <v>-4.1167927299999998E-5</v>
-      </c>
-      <c r="G24" s="1">
-        <v>-3.9167392099999998E-3</v>
-      </c>
-      <c r="H24" s="1">
-        <v>-2.4497542300000001E-3</v>
-      </c>
-      <c r="I24" s="1">
-        <v>4.04186558E-4</v>
-      </c>
-      <c r="J24" s="1">
-        <v>-4.7615246300000002E-4</v>
-      </c>
-      <c r="K24" s="1">
-        <v>5.5026991400000001E-3</v>
-      </c>
-      <c r="L24" s="1">
-        <v>0.29028538199999998</v>
-      </c>
-      <c r="M24" s="1">
+      <c r="C25" s="14">
+        <v>1.1064956600000001E-3</v>
+      </c>
+      <c r="D25" s="14">
+        <v>-7.60085707E-2</v>
+      </c>
+      <c r="E25" s="14">
+        <v>0.100657026</v>
+      </c>
+      <c r="F25" s="14">
+        <v>-3.9680319499999997E-5</v>
+      </c>
+      <c r="G25" s="14">
+        <v>-3.7752073899999998E-3</v>
+      </c>
+      <c r="H25" s="14">
+        <v>-2.3612320800000001E-3</v>
+      </c>
+      <c r="I25" s="14">
+        <v>3.8958123100000001E-4</v>
+      </c>
+      <c r="J25" s="14">
+        <v>-4.58946639E-4</v>
+      </c>
+      <c r="K25" s="14">
+        <v>5.3038584799999997E-3</v>
+      </c>
+      <c r="L25" s="14">
+        <v>0.31593100099999999</v>
+      </c>
+      <c r="M25" s="14">
         <v>0.99054363000000001</v>
       </c>
-      <c r="O24" s="1">
-        <f>C24*C8+D24*C7+E24*C6+ F24 * C8^2+G24*C7^2+H24*C6^2+I24*C8*C7+J24*C8*C6+K24*C6*C7+L24</f>
-        <v>0.99774151063289995</v>
-      </c>
+      <c r="O25" s="1">
+        <f>C25*C8+D25*C7+E25*C6+ F25 * C8^2+G25*C7^2+H25*C6^2+I25*C8*C7+J25*C8*C6+K25*C6*C7+L25</f>
+        <v>0.99782312669479989</v>
+      </c>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C30" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -632,7 +688,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -653,10 +709,19 @@
         <v>5</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>29</v>
+      <c r="E1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -670,9 +735,20 @@
         <v>7190</v>
       </c>
       <c r="D2" s="3">
+        <f>C2+230</f>
+        <v>7420</v>
+      </c>
+      <c r="E2" s="3">
         <v>1958</v>
       </c>
-      <c r="G2" s="5"/>
+      <c r="F2" s="3">
+        <f>E2-230-108</f>
+        <v>1620</v>
+      </c>
+      <c r="G2" s="6">
+        <f>E2-230</f>
+        <v>1728</v>
+      </c>
       <c r="H2" s="6"/>
       <c r="I2" s="5"/>
     </row>
@@ -687,9 +763,20 @@
         <v>7776</v>
       </c>
       <c r="D3" s="3">
+        <f t="shared" ref="D3:D25" si="0">C3+230</f>
+        <v>8006</v>
+      </c>
+      <c r="E3" s="3">
         <v>1998</v>
       </c>
-      <c r="G3" s="5"/>
+      <c r="F3" s="3">
+        <f t="shared" ref="F3:F25" si="1">E3-230-108</f>
+        <v>1660</v>
+      </c>
+      <c r="G3" s="6">
+        <f t="shared" ref="G3:G25" si="2">E3-230</f>
+        <v>1768</v>
+      </c>
       <c r="H3" s="6"/>
       <c r="I3" s="5"/>
     </row>
@@ -704,9 +791,20 @@
         <v>8420</v>
       </c>
       <c r="D4" s="3">
+        <f t="shared" si="0"/>
+        <v>8650</v>
+      </c>
+      <c r="E4" s="3">
         <v>2048</v>
       </c>
-      <c r="G4" s="5"/>
+      <c r="F4" s="3">
+        <f t="shared" si="1"/>
+        <v>1710</v>
+      </c>
+      <c r="G4" s="6">
+        <f t="shared" si="2"/>
+        <v>1818</v>
+      </c>
       <c r="H4" s="6"/>
       <c r="I4" s="5"/>
     </row>
@@ -721,9 +819,20 @@
         <v>9065</v>
       </c>
       <c r="D5" s="3">
+        <f t="shared" si="0"/>
+        <v>9295</v>
+      </c>
+      <c r="E5" s="3">
         <v>2098</v>
       </c>
-      <c r="G5" s="5"/>
+      <c r="F5" s="3">
+        <f t="shared" si="1"/>
+        <v>1760</v>
+      </c>
+      <c r="G5" s="6">
+        <f t="shared" si="2"/>
+        <v>1868</v>
+      </c>
       <c r="H5" s="6"/>
       <c r="I5" s="5"/>
     </row>
@@ -738,9 +847,20 @@
         <v>7014</v>
       </c>
       <c r="D6" s="3">
+        <f t="shared" si="0"/>
+        <v>7244</v>
+      </c>
+      <c r="E6" s="3">
         <v>2028</v>
       </c>
-      <c r="G6" s="5"/>
+      <c r="F6" s="3">
+        <f t="shared" si="1"/>
+        <v>1690</v>
+      </c>
+      <c r="G6" s="6">
+        <f t="shared" si="2"/>
+        <v>1798</v>
+      </c>
       <c r="H6" s="6"/>
       <c r="I6" s="5"/>
     </row>
@@ -755,9 +875,20 @@
         <v>7570</v>
       </c>
       <c r="D7" s="3">
+        <f t="shared" si="0"/>
+        <v>7800</v>
+      </c>
+      <c r="E7" s="3">
         <v>2078</v>
       </c>
-      <c r="G7" s="5"/>
+      <c r="F7" s="3">
+        <f t="shared" si="1"/>
+        <v>1740</v>
+      </c>
+      <c r="G7" s="6">
+        <f t="shared" si="2"/>
+        <v>1848</v>
+      </c>
       <c r="H7" s="6"/>
       <c r="I7" s="5"/>
     </row>
@@ -772,9 +903,20 @@
         <v>8186</v>
       </c>
       <c r="D8" s="3">
+        <f t="shared" si="0"/>
+        <v>8416</v>
+      </c>
+      <c r="E8" s="3">
         <v>2128</v>
       </c>
-      <c r="G8" s="5"/>
+      <c r="F8" s="3">
+        <f t="shared" si="1"/>
+        <v>1790</v>
+      </c>
+      <c r="G8" s="6">
+        <f t="shared" si="2"/>
+        <v>1898</v>
+      </c>
       <c r="H8" s="6"/>
       <c r="I8" s="5"/>
     </row>
@@ -789,9 +931,20 @@
         <v>8801</v>
       </c>
       <c r="D9" s="3">
+        <f t="shared" si="0"/>
+        <v>9031</v>
+      </c>
+      <c r="E9" s="3">
         <v>2178</v>
       </c>
-      <c r="G9" s="5"/>
+      <c r="F9" s="3">
+        <f t="shared" si="1"/>
+        <v>1840</v>
+      </c>
+      <c r="G9" s="6">
+        <f t="shared" si="2"/>
+        <v>1948</v>
+      </c>
       <c r="H9" s="6"/>
       <c r="I9" s="5"/>
     </row>
@@ -806,9 +959,20 @@
         <v>6809</v>
       </c>
       <c r="D10" s="3">
+        <f t="shared" si="0"/>
+        <v>7039</v>
+      </c>
+      <c r="E10" s="3">
         <v>2108</v>
       </c>
-      <c r="G10" s="5"/>
+      <c r="F10" s="3">
+        <f t="shared" si="1"/>
+        <v>1770</v>
+      </c>
+      <c r="G10" s="6">
+        <f t="shared" si="2"/>
+        <v>1878</v>
+      </c>
       <c r="H10" s="6"/>
       <c r="I10" s="5"/>
     </row>
@@ -823,9 +987,20 @@
         <v>7365</v>
       </c>
       <c r="D11" s="3">
+        <f t="shared" si="0"/>
+        <v>7595</v>
+      </c>
+      <c r="E11" s="3">
         <v>2148</v>
       </c>
-      <c r="G11" s="5"/>
+      <c r="F11" s="3">
+        <f t="shared" si="1"/>
+        <v>1810</v>
+      </c>
+      <c r="G11" s="6">
+        <f t="shared" si="2"/>
+        <v>1918</v>
+      </c>
       <c r="H11" s="6"/>
       <c r="I11" s="5"/>
     </row>
@@ -839,10 +1014,21 @@
       <c r="C12" s="8">
         <v>7951</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="11">
+        <f t="shared" si="0"/>
+        <v>8181</v>
+      </c>
+      <c r="E12" s="8">
         <v>2196</v>
       </c>
-      <c r="G12" s="5"/>
+      <c r="F12" s="11">
+        <f t="shared" si="1"/>
+        <v>1858</v>
+      </c>
+      <c r="G12" s="12">
+        <f t="shared" si="2"/>
+        <v>1966</v>
+      </c>
       <c r="H12" s="6"/>
       <c r="I12" s="5"/>
     </row>
@@ -857,9 +1043,20 @@
         <v>8567</v>
       </c>
       <c r="D13" s="3">
+        <f t="shared" si="0"/>
+        <v>8797</v>
+      </c>
+      <c r="E13" s="3">
         <v>2248</v>
       </c>
-      <c r="G13" s="5"/>
+      <c r="F13" s="3">
+        <f t="shared" si="1"/>
+        <v>1910</v>
+      </c>
+      <c r="G13" s="6">
+        <f t="shared" si="2"/>
+        <v>2018</v>
+      </c>
       <c r="H13" s="6"/>
       <c r="I13" s="5"/>
     </row>
@@ -874,9 +1071,20 @@
         <v>6633</v>
       </c>
       <c r="D14" s="3">
+        <f t="shared" si="0"/>
+        <v>6863</v>
+      </c>
+      <c r="E14" s="3">
         <v>2188</v>
       </c>
-      <c r="G14" s="5"/>
+      <c r="F14" s="3">
+        <f t="shared" si="1"/>
+        <v>1850</v>
+      </c>
+      <c r="G14" s="6">
+        <f t="shared" si="2"/>
+        <v>1958</v>
+      </c>
       <c r="H14" s="6"/>
       <c r="I14" s="5"/>
     </row>
@@ -891,9 +1099,20 @@
         <v>7160</v>
       </c>
       <c r="D15" s="3">
+        <f t="shared" si="0"/>
+        <v>7390</v>
+      </c>
+      <c r="E15" s="3">
         <v>2228</v>
       </c>
-      <c r="G15" s="5"/>
+      <c r="F15" s="3">
+        <f t="shared" si="1"/>
+        <v>1890</v>
+      </c>
+      <c r="G15" s="6">
+        <f t="shared" si="2"/>
+        <v>1998</v>
+      </c>
       <c r="H15" s="6"/>
       <c r="I15" s="5"/>
     </row>
@@ -908,9 +1127,20 @@
         <v>7717</v>
       </c>
       <c r="D16" s="3">
+        <f t="shared" si="0"/>
+        <v>7947</v>
+      </c>
+      <c r="E16" s="3">
         <v>2278</v>
       </c>
-      <c r="G16" s="5"/>
+      <c r="F16" s="3">
+        <f t="shared" si="1"/>
+        <v>1940</v>
+      </c>
+      <c r="G16" s="6">
+        <f t="shared" si="2"/>
+        <v>2048</v>
+      </c>
       <c r="H16" s="6"/>
       <c r="I16" s="5"/>
     </row>
@@ -925,9 +1155,20 @@
         <v>8274</v>
       </c>
       <c r="D17" s="3">
+        <f t="shared" si="0"/>
+        <v>8504</v>
+      </c>
+      <c r="E17" s="3">
         <v>2318</v>
       </c>
-      <c r="G17" s="5"/>
+      <c r="F17" s="3">
+        <f t="shared" si="1"/>
+        <v>1980</v>
+      </c>
+      <c r="G17" s="6">
+        <f t="shared" si="2"/>
+        <v>2088</v>
+      </c>
       <c r="H17" s="6"/>
       <c r="I17" s="5"/>
     </row>
@@ -942,9 +1183,20 @@
         <v>6428</v>
       </c>
       <c r="D18" s="3">
+        <f t="shared" si="0"/>
+        <v>6658</v>
+      </c>
+      <c r="E18" s="3">
         <v>2278</v>
       </c>
-      <c r="G18" s="5"/>
+      <c r="F18" s="3">
+        <f t="shared" si="1"/>
+        <v>1940</v>
+      </c>
+      <c r="G18" s="6">
+        <f t="shared" si="2"/>
+        <v>2048</v>
+      </c>
       <c r="H18" s="6"/>
       <c r="I18" s="5"/>
     </row>
@@ -959,9 +1211,20 @@
         <v>6926</v>
       </c>
       <c r="D19" s="3">
+        <f t="shared" si="0"/>
+        <v>7156</v>
+      </c>
+      <c r="E19" s="3">
         <v>2318</v>
       </c>
-      <c r="G19" s="5"/>
+      <c r="F19" s="3">
+        <f t="shared" si="1"/>
+        <v>1980</v>
+      </c>
+      <c r="G19" s="6">
+        <f t="shared" si="2"/>
+        <v>2088</v>
+      </c>
       <c r="H19" s="6"/>
       <c r="I19" s="5"/>
     </row>
@@ -976,9 +1239,20 @@
         <v>7453</v>
       </c>
       <c r="D20" s="3">
+        <f t="shared" si="0"/>
+        <v>7683</v>
+      </c>
+      <c r="E20" s="3">
         <v>2358</v>
       </c>
-      <c r="G20" s="5"/>
+      <c r="F20" s="3">
+        <f t="shared" si="1"/>
+        <v>2020</v>
+      </c>
+      <c r="G20" s="6">
+        <f t="shared" si="2"/>
+        <v>2128</v>
+      </c>
       <c r="H20" s="6"/>
       <c r="I20" s="5"/>
     </row>
@@ -993,9 +1267,20 @@
         <v>8010</v>
       </c>
       <c r="D21" s="3">
+        <f t="shared" si="0"/>
+        <v>8240</v>
+      </c>
+      <c r="E21" s="3">
         <v>2398</v>
       </c>
-      <c r="G21" s="5"/>
+      <c r="F21" s="3">
+        <f t="shared" si="1"/>
+        <v>2060</v>
+      </c>
+      <c r="G21" s="6">
+        <f t="shared" si="2"/>
+        <v>2168</v>
+      </c>
       <c r="H21" s="6"/>
       <c r="I21" s="5"/>
     </row>
@@ -1010,9 +1295,20 @@
         <v>6018</v>
       </c>
       <c r="D22" s="3">
+        <f t="shared" si="0"/>
+        <v>6248</v>
+      </c>
+      <c r="E22" s="3">
         <v>2448</v>
       </c>
-      <c r="G22" s="5"/>
+      <c r="F22" s="3">
+        <f t="shared" si="1"/>
+        <v>2110</v>
+      </c>
+      <c r="G22" s="6">
+        <f t="shared" si="2"/>
+        <v>2218</v>
+      </c>
       <c r="H22" s="6"/>
       <c r="I22" s="5"/>
     </row>
@@ -1027,9 +1323,20 @@
         <v>6486</v>
       </c>
       <c r="D23" s="3">
+        <f t="shared" si="0"/>
+        <v>6716</v>
+      </c>
+      <c r="E23" s="3">
         <v>2478</v>
       </c>
-      <c r="G23" s="5"/>
+      <c r="F23" s="3">
+        <f t="shared" si="1"/>
+        <v>2140</v>
+      </c>
+      <c r="G23" s="6">
+        <f t="shared" si="2"/>
+        <v>2248</v>
+      </c>
       <c r="H23" s="6"/>
       <c r="I23" s="5"/>
     </row>
@@ -1044,9 +1351,20 @@
         <v>6984</v>
       </c>
       <c r="D24" s="3">
+        <f t="shared" si="0"/>
+        <v>7214</v>
+      </c>
+      <c r="E24" s="3">
         <v>2518</v>
       </c>
-      <c r="G24" s="5"/>
+      <c r="F24" s="3">
+        <f t="shared" si="1"/>
+        <v>2180</v>
+      </c>
+      <c r="G24" s="6">
+        <f t="shared" si="2"/>
+        <v>2288</v>
+      </c>
       <c r="H24" s="6"/>
       <c r="I24" s="5"/>
     </row>
@@ -1061,9 +1379,20 @@
         <v>7483</v>
       </c>
       <c r="D25" s="3">
+        <f t="shared" si="0"/>
+        <v>7713</v>
+      </c>
+      <c r="E25" s="3">
         <v>2548</v>
       </c>
-      <c r="G25" s="5"/>
+      <c r="F25" s="3">
+        <f t="shared" si="1"/>
+        <v>2210</v>
+      </c>
+      <c r="G25" s="6">
+        <f t="shared" si="2"/>
+        <v>2318</v>
+      </c>
       <c r="H25" s="6"/>
       <c r="I25" s="5"/>
     </row>
@@ -1082,10 +1411,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D121"/>
+  <dimension ref="A1:E121"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G55" sqref="G55"/>
+    <sheetView topLeftCell="A18" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1093,7 +1422,7 @@
     <col min="1" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -1104,10 +1433,13 @@
         <v>3</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>29.4</v>
       </c>
@@ -1120,8 +1452,12 @@
       <c r="D2" s="6">
         <v>6311</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" s="6">
+        <f>D2+230</f>
+        <v>6541</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>29.4</v>
       </c>
@@ -1134,8 +1470,12 @@
       <c r="D3" s="6">
         <v>6867</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" s="6">
+        <f t="shared" ref="E3:E66" si="0">D3+230</f>
+        <v>7097</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>29.4</v>
       </c>
@@ -1148,8 +1488,12 @@
       <c r="D4" s="6">
         <v>7277</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" s="6">
+        <f t="shared" si="0"/>
+        <v>7507</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>29.4</v>
       </c>
@@ -1162,8 +1506,12 @@
       <c r="D5" s="6">
         <v>7483</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" s="6">
+        <f t="shared" si="0"/>
+        <v>7713</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>29.4</v>
       </c>
@@ -1176,8 +1524,12 @@
       <c r="D6" s="6">
         <v>7658</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" s="6">
+        <f t="shared" si="0"/>
+        <v>7888</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>29.4</v>
       </c>
@@ -1190,8 +1542,12 @@
       <c r="D7" s="6">
         <v>5256</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" s="6">
+        <f t="shared" si="0"/>
+        <v>5486</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>29.4</v>
       </c>
@@ -1204,8 +1560,12 @@
       <c r="D8" s="6">
         <v>5812</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" s="6">
+        <f t="shared" si="0"/>
+        <v>6042</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>29.4</v>
       </c>
@@ -1218,8 +1578,12 @@
       <c r="D9" s="6">
         <v>6369</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" s="6">
+        <f t="shared" si="0"/>
+        <v>6599</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>29.4</v>
       </c>
@@ -1232,8 +1596,12 @@
       <c r="D10" s="6">
         <v>6897</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" s="6">
+        <f t="shared" si="0"/>
+        <v>7127</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>29.4</v>
       </c>
@@ -1246,8 +1614,12 @@
       <c r="D11" s="6">
         <v>7453</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" s="6">
+        <f t="shared" si="0"/>
+        <v>7683</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>29.4</v>
       </c>
@@ -1260,8 +1632,12 @@
       <c r="D12" s="6">
         <v>4113</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" s="6">
+        <f t="shared" si="0"/>
+        <v>4343</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>29.4</v>
       </c>
@@ -1274,8 +1650,12 @@
       <c r="D13" s="6">
         <v>4670</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13" s="6">
+        <f t="shared" si="0"/>
+        <v>4900</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>29.4</v>
       </c>
@@ -1288,8 +1668,12 @@
       <c r="D14" s="6">
         <v>5226</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14" s="6">
+        <f t="shared" si="0"/>
+        <v>5456</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>29.4</v>
       </c>
@@ -1302,8 +1686,12 @@
       <c r="D15" s="6">
         <v>5754</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15" s="6">
+        <f t="shared" si="0"/>
+        <v>5984</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>29.4</v>
       </c>
@@ -1316,8 +1704,12 @@
       <c r="D16" s="6">
         <v>6311</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" s="6">
+        <f t="shared" si="0"/>
+        <v>6541</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>29.4</v>
       </c>
@@ -1330,8 +1722,12 @@
       <c r="D17" s="6">
         <v>2970</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" s="6">
+        <f t="shared" si="0"/>
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>29.4</v>
       </c>
@@ -1344,8 +1740,12 @@
       <c r="D18" s="6">
         <v>3498</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" s="6">
+        <f t="shared" si="0"/>
+        <v>3728</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>29.4</v>
       </c>
@@ -1358,8 +1758,12 @@
       <c r="D19" s="6">
         <v>4054</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19" s="6">
+        <f t="shared" si="0"/>
+        <v>4284</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>29.4</v>
       </c>
@@ -1372,8 +1776,12 @@
       <c r="D20" s="6">
         <v>4582</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20" s="6">
+        <f t="shared" si="0"/>
+        <v>4812</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>29.4</v>
       </c>
@@ -1386,8 +1794,12 @@
       <c r="D21" s="6">
         <v>5139</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" s="6">
+        <f t="shared" si="0"/>
+        <v>5369</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>32.200000000000003</v>
       </c>
@@ -1400,8 +1812,12 @@
       <c r="D22" s="6">
         <v>6223</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22" s="6">
+        <f t="shared" si="0"/>
+        <v>6453</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <v>32.200000000000003</v>
       </c>
@@ -1414,8 +1830,12 @@
       <c r="D23" s="6">
         <v>6779</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23" s="6">
+        <f t="shared" si="0"/>
+        <v>7009</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>32.200000000000003</v>
       </c>
@@ -1428,8 +1848,12 @@
       <c r="D24" s="6">
         <v>7131</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24" s="6">
+        <f t="shared" si="0"/>
+        <v>7361</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>32.200000000000003</v>
       </c>
@@ -1442,8 +1866,12 @@
       <c r="D25" s="6">
         <v>7307</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25" s="6">
+        <f t="shared" si="0"/>
+        <v>7537</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>32.200000000000003</v>
       </c>
@@ -1456,8 +1884,12 @@
       <c r="D26" s="6">
         <v>7512</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E26" s="6">
+        <f t="shared" si="0"/>
+        <v>7742</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <v>32.200000000000003</v>
       </c>
@@ -1470,8 +1902,12 @@
       <c r="D27" s="6">
         <v>5197</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E27" s="6">
+        <f t="shared" si="0"/>
+        <v>5427</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <v>32.200000000000003</v>
       </c>
@@ -1484,8 +1920,12 @@
       <c r="D28" s="6">
         <v>5725</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E28" s="6">
+        <f t="shared" si="0"/>
+        <v>5955</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
         <v>32.200000000000003</v>
       </c>
@@ -1498,8 +1938,12 @@
       <c r="D29" s="6">
         <v>6281</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E29" s="6">
+        <f t="shared" si="0"/>
+        <v>6511</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <v>32.200000000000003</v>
       </c>
@@ -1512,8 +1956,12 @@
       <c r="D30" s="6">
         <v>6809</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E30" s="6">
+        <f t="shared" si="0"/>
+        <v>7039</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <v>32.200000000000003</v>
       </c>
@@ -1526,8 +1974,12 @@
       <c r="D31" s="6">
         <v>7365</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E31" s="6">
+        <f t="shared" si="0"/>
+        <v>7595</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
         <v>32.200000000000003</v>
       </c>
@@ -1540,8 +1992,12 @@
       <c r="D32" s="6">
         <v>4025</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32" s="6">
+        <f t="shared" si="0"/>
+        <v>4255</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
         <v>32.200000000000003</v>
       </c>
@@ -1554,8 +2010,12 @@
       <c r="D33" s="6">
         <v>4582</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E33" s="6">
+        <f t="shared" si="0"/>
+        <v>4812</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <v>32.200000000000003</v>
       </c>
@@ -1568,8 +2028,12 @@
       <c r="D34" s="6">
         <v>5139</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E34" s="6">
+        <f t="shared" si="0"/>
+        <v>5369</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
         <v>32.200000000000003</v>
       </c>
@@ -1582,8 +2046,12 @@
       <c r="D35" s="6">
         <v>5666</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E35" s="6">
+        <f t="shared" si="0"/>
+        <v>5896</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
         <v>32.200000000000003</v>
       </c>
@@ -1596,8 +2064,12 @@
       <c r="D36" s="6">
         <v>6223</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E36" s="6">
+        <f t="shared" si="0"/>
+        <v>6453</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
         <v>32.200000000000003</v>
       </c>
@@ -1610,8 +2082,12 @@
       <c r="D37" s="6">
         <v>2853</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E37" s="6">
+        <f t="shared" si="0"/>
+        <v>3083</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
         <v>32.200000000000003</v>
       </c>
@@ -1624,8 +2100,12 @@
       <c r="D38" s="6">
         <v>3410</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E38" s="6">
+        <f t="shared" si="0"/>
+        <v>3640</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="4">
         <v>32.200000000000003</v>
       </c>
@@ -1638,8 +2118,12 @@
       <c r="D39" s="6">
         <v>3967</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E39" s="6">
+        <f t="shared" si="0"/>
+        <v>4197</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
         <v>32.200000000000003</v>
       </c>
@@ -1652,8 +2136,12 @@
       <c r="D40" s="6">
         <v>4494</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E40" s="6">
+        <f t="shared" si="0"/>
+        <v>4724</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="4">
         <v>32.200000000000003</v>
       </c>
@@ -1666,8 +2154,12 @@
       <c r="D41" s="6">
         <v>5051</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E41" s="6">
+        <f t="shared" si="0"/>
+        <v>5281</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
         <v>35</v>
       </c>
@@ -1680,8 +2172,12 @@
       <c r="D42" s="6">
         <v>6164</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E42" s="6">
+        <f t="shared" si="0"/>
+        <v>6394</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
         <v>35</v>
       </c>
@@ -1694,8 +2190,12 @@
       <c r="D43" s="6">
         <v>6691</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E43" s="6">
+        <f t="shared" si="0"/>
+        <v>6921</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="4">
         <v>35</v>
       </c>
@@ -1708,8 +2208,12 @@
       <c r="D44" s="6">
         <v>6984</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E44" s="6">
+        <f t="shared" si="0"/>
+        <v>7214</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="4">
         <v>35</v>
       </c>
@@ -1722,8 +2226,12 @@
       <c r="D45" s="6">
         <v>7160</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E45" s="6">
+        <f t="shared" si="0"/>
+        <v>7390</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="4">
         <v>35</v>
       </c>
@@ -1736,8 +2244,12 @@
       <c r="D46" s="6">
         <v>7336</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E46" s="6">
+        <f t="shared" si="0"/>
+        <v>7566</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="4">
         <v>35</v>
       </c>
@@ -1750,8 +2262,12 @@
       <c r="D47" s="6">
         <v>5109</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E47" s="6">
+        <f t="shared" si="0"/>
+        <v>5339</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="4">
         <v>35</v>
       </c>
@@ -1764,8 +2280,12 @@
       <c r="D48" s="6">
         <v>5637</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E48" s="6">
+        <f t="shared" si="0"/>
+        <v>5867</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="4">
         <v>35</v>
       </c>
@@ -1778,8 +2298,12 @@
       <c r="D49" s="6">
         <v>6193</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E49" s="6">
+        <f t="shared" si="0"/>
+        <v>6423</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="4">
         <v>35</v>
       </c>
@@ -1792,8 +2316,12 @@
       <c r="D50" s="6">
         <v>6721</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E50" s="6">
+        <f t="shared" si="0"/>
+        <v>6951</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="4">
         <v>35</v>
       </c>
@@ -1806,8 +2334,12 @@
       <c r="D51" s="6">
         <v>7277</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E51" s="6">
+        <f t="shared" si="0"/>
+        <v>7507</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
         <v>35</v>
       </c>
@@ -1820,8 +2352,12 @@
       <c r="D52" s="6">
         <v>3937</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E52" s="6">
+        <f t="shared" si="0"/>
+        <v>4167</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
         <v>35</v>
       </c>
@@ -1834,8 +2370,12 @@
       <c r="D53" s="6">
         <v>4494</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E53" s="6">
+        <f t="shared" si="0"/>
+        <v>4724</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="4">
         <v>35</v>
       </c>
@@ -1848,8 +2388,12 @@
       <c r="D54" s="6">
         <v>5051</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E54" s="6">
+        <f t="shared" si="0"/>
+        <v>5281</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="4">
         <v>35</v>
       </c>
@@ -1862,8 +2406,12 @@
       <c r="D55" s="6">
         <v>5578</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E55" s="6">
+        <f t="shared" si="0"/>
+        <v>5808</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="7">
         <v>35</v>
       </c>
@@ -1876,8 +2424,12 @@
       <c r="D56" s="9">
         <v>6135</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E56" s="12">
+        <f t="shared" si="0"/>
+        <v>6365</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="4">
         <v>35</v>
       </c>
@@ -1890,8 +2442,12 @@
       <c r="D57" s="6">
         <v>2765</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E57" s="6">
+        <f t="shared" si="0"/>
+        <v>2995</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="4">
         <v>35</v>
       </c>
@@ -1904,8 +2460,12 @@
       <c r="D58" s="6">
         <v>3322</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E58" s="6">
+        <f t="shared" si="0"/>
+        <v>3552</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="4">
         <v>35</v>
       </c>
@@ -1918,8 +2478,12 @@
       <c r="D59" s="6">
         <v>3849</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E59" s="6">
+        <f t="shared" si="0"/>
+        <v>4079</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="4">
         <v>35</v>
       </c>
@@ -1932,8 +2496,12 @@
       <c r="D60" s="6">
         <v>4406</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E60" s="6">
+        <f t="shared" si="0"/>
+        <v>4636</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="4">
         <v>35</v>
       </c>
@@ -1946,8 +2514,12 @@
       <c r="D61" s="6">
         <v>4963</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E61" s="6">
+        <f t="shared" si="0"/>
+        <v>5193</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="4">
         <v>37.799999999999997</v>
       </c>
@@ -1960,8 +2532,12 @@
       <c r="D62" s="6">
         <v>6076</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E62" s="6">
+        <f t="shared" si="0"/>
+        <v>6306</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="4">
         <v>37.799999999999997</v>
       </c>
@@ -1974,8 +2550,12 @@
       <c r="D63" s="6">
         <v>6633</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E63" s="6">
+        <f t="shared" si="0"/>
+        <v>6863</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="4">
         <v>37.799999999999997</v>
       </c>
@@ -1988,8 +2568,12 @@
       <c r="D64" s="6">
         <v>6809</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E64" s="6">
+        <f t="shared" si="0"/>
+        <v>7039</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="4">
         <v>37.799999999999997</v>
       </c>
@@ -2002,8 +2586,12 @@
       <c r="D65" s="6">
         <v>6984</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E65" s="6">
+        <f t="shared" si="0"/>
+        <v>7214</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="4">
         <v>37.799999999999997</v>
       </c>
@@ -2016,8 +2604,12 @@
       <c r="D66" s="6">
         <v>7160</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E66" s="6">
+        <f t="shared" si="0"/>
+        <v>7390</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="4">
         <v>37.799999999999997</v>
       </c>
@@ -2030,8 +2622,12 @@
       <c r="D67" s="6">
         <v>5021</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E67" s="6">
+        <f t="shared" ref="E67:E121" si="1">D67+230</f>
+        <v>5251</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="4">
         <v>37.799999999999997</v>
       </c>
@@ -2044,8 +2640,12 @@
       <c r="D68" s="6">
         <v>5549</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E68" s="6">
+        <f t="shared" si="1"/>
+        <v>5779</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="4">
         <v>37.799999999999997</v>
       </c>
@@ -2058,8 +2658,12 @@
       <c r="D69" s="6">
         <v>6105</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E69" s="6">
+        <f t="shared" si="1"/>
+        <v>6335</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="4">
         <v>37.799999999999997</v>
       </c>
@@ -2072,8 +2676,12 @@
       <c r="D70" s="6">
         <v>6633</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E70" s="6">
+        <f t="shared" si="1"/>
+        <v>6863</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="4">
         <v>37.799999999999997</v>
       </c>
@@ -2086,8 +2694,12 @@
       <c r="D71" s="6">
         <v>7160</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E71" s="6">
+        <f t="shared" si="1"/>
+        <v>7390</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="4">
         <v>37.799999999999997</v>
       </c>
@@ -2100,8 +2712,12 @@
       <c r="D72" s="6">
         <v>3849</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E72" s="6">
+        <f t="shared" si="1"/>
+        <v>4079</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="4">
         <v>37.799999999999997</v>
       </c>
@@ -2114,8 +2730,12 @@
       <c r="D73" s="6">
         <v>4406</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E73" s="6">
+        <f t="shared" si="1"/>
+        <v>4636</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="4">
         <v>37.799999999999997</v>
       </c>
@@ -2128,8 +2748,12 @@
       <c r="D74" s="6">
         <v>4933</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E74" s="6">
+        <f t="shared" si="1"/>
+        <v>5163</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="4">
         <v>37.799999999999997</v>
       </c>
@@ -2142,8 +2766,12 @@
       <c r="D75" s="6">
         <v>5490</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E75" s="6">
+        <f t="shared" si="1"/>
+        <v>5720</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="4">
         <v>37.799999999999997</v>
       </c>
@@ -2156,8 +2784,12 @@
       <c r="D76" s="6">
         <v>6047</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E76" s="6">
+        <f t="shared" si="1"/>
+        <v>6277</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="4">
         <v>37.799999999999997</v>
       </c>
@@ -2170,8 +2802,12 @@
       <c r="D77" s="6">
         <v>2677</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E77" s="6">
+        <f t="shared" si="1"/>
+        <v>2907</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="4">
         <v>37.799999999999997</v>
       </c>
@@ -2184,8 +2820,12 @@
       <c r="D78" s="6">
         <v>3234</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E78" s="6">
+        <f t="shared" si="1"/>
+        <v>3464</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="4">
         <v>37.799999999999997</v>
       </c>
@@ -2198,8 +2838,12 @@
       <c r="D79" s="6">
         <v>3761</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E79" s="6">
+        <f t="shared" si="1"/>
+        <v>3991</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="4">
         <v>37.799999999999997</v>
       </c>
@@ -2212,8 +2856,12 @@
       <c r="D80" s="6">
         <v>4318</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E80" s="6">
+        <f t="shared" si="1"/>
+        <v>4548</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="4">
         <v>37.799999999999997</v>
       </c>
@@ -2226,8 +2874,12 @@
       <c r="D81" s="6">
         <v>4846</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E81" s="6">
+        <f t="shared" si="1"/>
+        <v>5076</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="4">
         <v>40.6</v>
       </c>
@@ -2240,8 +2892,12 @@
       <c r="D82" s="6">
         <v>5988</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E82" s="6">
+        <f t="shared" si="1"/>
+        <v>6218</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="4">
         <v>40.6</v>
       </c>
@@ -2254,8 +2910,12 @@
       <c r="D83" s="6">
         <v>6486</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E83" s="6">
+        <f t="shared" si="1"/>
+        <v>6716</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="4">
         <v>40.6</v>
       </c>
@@ -2268,8 +2928,12 @@
       <c r="D84" s="6">
         <v>6633</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E84" s="6">
+        <f t="shared" si="1"/>
+        <v>6863</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="4">
         <v>40.6</v>
       </c>
@@ -2282,8 +2946,12 @@
       <c r="D85" s="6">
         <v>6809</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E85" s="6">
+        <f t="shared" si="1"/>
+        <v>7039</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="4">
         <v>40.6</v>
       </c>
@@ -2296,8 +2964,12 @@
       <c r="D86" s="6">
         <v>6984</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E86" s="6">
+        <f t="shared" si="1"/>
+        <v>7214</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="4">
         <v>40.6</v>
       </c>
@@ -2310,8 +2982,12 @@
       <c r="D87" s="6">
         <v>4933</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E87" s="6">
+        <f t="shared" si="1"/>
+        <v>5163</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="4">
         <v>40.6</v>
       </c>
@@ -2324,8 +3000,12 @@
       <c r="D88" s="6">
         <v>5461</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E88" s="6">
+        <f t="shared" si="1"/>
+        <v>5691</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="4">
         <v>40.6</v>
       </c>
@@ -2338,8 +3018,12 @@
       <c r="D89" s="6">
         <v>6018</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E89" s="6">
+        <f t="shared" si="1"/>
+        <v>6248</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="4">
         <v>40.6</v>
       </c>
@@ -2352,8 +3036,12 @@
       <c r="D90" s="6">
         <v>6545</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E90" s="6">
+        <f t="shared" si="1"/>
+        <v>6775</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="4">
         <v>40.6</v>
       </c>
@@ -2366,8 +3054,12 @@
       <c r="D91" s="6">
         <v>6984</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E91" s="6">
+        <f t="shared" si="1"/>
+        <v>7214</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="4">
         <v>40.6</v>
       </c>
@@ -2380,8 +3072,12 @@
       <c r="D92" s="6">
         <v>3761</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E92" s="6">
+        <f t="shared" si="1"/>
+        <v>3991</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" s="4">
         <v>40.6</v>
       </c>
@@ -2394,8 +3090,12 @@
       <c r="D93" s="6">
         <v>4318</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E93" s="6">
+        <f t="shared" si="1"/>
+        <v>4548</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="4">
         <v>40.6</v>
       </c>
@@ -2408,8 +3108,12 @@
       <c r="D94" s="6">
         <v>4846</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E94" s="6">
+        <f t="shared" si="1"/>
+        <v>5076</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="4">
         <v>40.6</v>
       </c>
@@ -2422,8 +3126,12 @@
       <c r="D95" s="6">
         <v>5402</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E95" s="6">
+        <f t="shared" si="1"/>
+        <v>5632</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="4">
         <v>40.6</v>
       </c>
@@ -2436,8 +3144,12 @@
       <c r="D96" s="6">
         <v>5930</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E96" s="6">
+        <f t="shared" si="1"/>
+        <v>6160</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" s="4">
         <v>40.6</v>
       </c>
@@ -2450,8 +3162,12 @@
       <c r="D97" s="6">
         <v>2589</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E97" s="6">
+        <f t="shared" si="1"/>
+        <v>2819</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" s="4">
         <v>40.6</v>
       </c>
@@ -2464,8 +3180,12 @@
       <c r="D98" s="6">
         <v>3117</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E98" s="6">
+        <f t="shared" si="1"/>
+        <v>3347</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" s="4">
         <v>40.6</v>
       </c>
@@ -2478,8 +3198,12 @@
       <c r="D99" s="6">
         <v>3674</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E99" s="6">
+        <f t="shared" si="1"/>
+        <v>3904</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" s="4">
         <v>40.6</v>
       </c>
@@ -2492,8 +3216,12 @@
       <c r="D100" s="6">
         <v>4230</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E100" s="6">
+        <f t="shared" si="1"/>
+        <v>4460</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" s="4">
         <v>40.6</v>
       </c>
@@ -2506,8 +3234,12 @@
       <c r="D101" s="6">
         <v>4758</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E101" s="6">
+        <f t="shared" si="1"/>
+        <v>4988</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" s="4">
         <v>46.1</v>
       </c>
@@ -2520,8 +3252,12 @@
       <c r="D102" s="6">
         <v>5812</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E102" s="6">
+        <f t="shared" si="1"/>
+        <v>6042</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" s="4">
         <v>46.1</v>
       </c>
@@ -2534,8 +3270,12 @@
       <c r="D103" s="6">
         <v>6135</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E103" s="6">
+        <f t="shared" si="1"/>
+        <v>6365</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" s="4">
         <v>46.1</v>
       </c>
@@ -2548,8 +3288,12 @@
       <c r="D104" s="6">
         <v>6311</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E104" s="6">
+        <f t="shared" si="1"/>
+        <v>6541</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" s="4">
         <v>46.1</v>
       </c>
@@ -2562,8 +3306,12 @@
       <c r="D105" s="6">
         <v>6457</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E105" s="6">
+        <f t="shared" si="1"/>
+        <v>6687</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" s="4">
         <v>46.1</v>
       </c>
@@ -2576,8 +3324,12 @@
       <c r="D106" s="6">
         <v>6604</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E106" s="6">
+        <f t="shared" si="1"/>
+        <v>6834</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" s="4">
         <v>46.1</v>
       </c>
@@ -2590,8 +3342,12 @@
       <c r="D107" s="6">
         <v>4758</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E107" s="6">
+        <f t="shared" si="1"/>
+        <v>4988</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" s="4">
         <v>46.1</v>
       </c>
@@ -2604,8 +3360,12 @@
       <c r="D108" s="6">
         <v>5285</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E108" s="6">
+        <f t="shared" si="1"/>
+        <v>5515</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" s="4">
         <v>46.1</v>
       </c>
@@ -2618,8 +3378,12 @@
       <c r="D109" s="6">
         <v>5842</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E109" s="6">
+        <f t="shared" si="1"/>
+        <v>6072</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" s="4">
         <v>46.1</v>
       </c>
@@ -2632,8 +3396,12 @@
       <c r="D110" s="6">
         <v>6369</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E110" s="6">
+        <f t="shared" si="1"/>
+        <v>6599</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" s="4">
         <v>46.1</v>
       </c>
@@ -2646,8 +3414,12 @@
       <c r="D111" s="6">
         <v>6604</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E111" s="6">
+        <f t="shared" si="1"/>
+        <v>6834</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" s="4">
         <v>46.1</v>
       </c>
@@ -2660,8 +3432,12 @@
       <c r="D112" s="6">
         <v>3586</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E112" s="6">
+        <f t="shared" si="1"/>
+        <v>3816</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" s="4">
         <v>46.1</v>
       </c>
@@ -2674,8 +3450,12 @@
       <c r="D113" s="6">
         <v>4142</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E113" s="6">
+        <f t="shared" si="1"/>
+        <v>4372</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" s="4">
         <v>46.1</v>
       </c>
@@ -2688,8 +3468,12 @@
       <c r="D114" s="6">
         <v>4670</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E114" s="6">
+        <f t="shared" si="1"/>
+        <v>4900</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" s="4">
         <v>46.1</v>
       </c>
@@ -2702,8 +3486,12 @@
       <c r="D115" s="6">
         <v>5226</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E115" s="6">
+        <f t="shared" si="1"/>
+        <v>5456</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" s="4">
         <v>46.1</v>
       </c>
@@ -2716,8 +3504,12 @@
       <c r="D116" s="6">
         <v>5754</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E116" s="6">
+        <f t="shared" si="1"/>
+        <v>5984</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" s="4">
         <v>46.1</v>
       </c>
@@ -2730,8 +3522,12 @@
       <c r="D117" s="6">
         <v>2414</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E117" s="6">
+        <f t="shared" si="1"/>
+        <v>2644</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" s="4">
         <v>46.1</v>
       </c>
@@ -2744,8 +3540,12 @@
       <c r="D118" s="6">
         <v>2941</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E118" s="6">
+        <f t="shared" si="1"/>
+        <v>3171</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" s="4">
         <v>46.1</v>
       </c>
@@ -2758,8 +3558,12 @@
       <c r="D119" s="6">
         <v>3498</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E119" s="6">
+        <f t="shared" si="1"/>
+        <v>3728</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" s="4">
         <v>46.1</v>
       </c>
@@ -2772,8 +3576,12 @@
       <c r="D120" s="6">
         <v>4025</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E120" s="6">
+        <f t="shared" si="1"/>
+        <v>4255</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" s="4">
         <v>46.1</v>
       </c>
@@ -2785,6 +3593,10 @@
       </c>
       <c r="D121" s="6">
         <v>4582</v>
+      </c>
+      <c r="E121" s="6">
+        <f t="shared" si="1"/>
+        <v>4812</v>
       </c>
     </row>
   </sheetData>

</xml_diff>